<commit_message>
Add some changes in latex
</commit_message>
<xml_diff>
--- a/Document/Data/Data-Preparat.xlsx
+++ b/Document/Data/Data-Preparat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhammad Naufal\Downloads\Laprak\Laporan-Praktikum-Eksperimen-Fisika\Document\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC43B4CF-34C1-488B-86D9-550F0500136F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBEF2DF-7158-4E3D-9E0E-79C0B0DE086C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="2625" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Na-22" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4243" uniqueCount="13">
   <si>
     <t>n</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>n^2</t>
+  </si>
+  <si>
+    <t>ln^2(w.n!)</t>
+  </si>
+  <si>
+    <t>n.ln(w.n!)</t>
   </si>
 </sst>
 </file>
@@ -3412,495 +3418,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Am-241'!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ln(w.n!)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.17509908136482941"/>
-                  <c:y val="-7.9542140565762613E-4"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Am-241'!$F$2:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Am-241'!$K$2:$K$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>-1.8971199848858813</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.3318061758358208</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.53102833108351022</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.10975086395911929</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.33074156191222798</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5173226235262947</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7509374747077999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.3899948043230586</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D557-4467-8312-CE73928274AE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1886131151"/>
-        <c:axId val="1876191759"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1886131151"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1876191759"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1876191759"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1886131151"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3941,563 +3458,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5054,47 +4015,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE4F067-769F-4CE9-8933-D2326054144F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5358,10 +4278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K171"/>
+  <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5369,7 +4289,7 @@
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5403,8 +4323,14 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5442,8 +4368,16 @@
         <f>LN(J2*H2)</f>
         <v>-1.7719568419318752</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>(K2)^2</f>
+        <v>3.1398310496691844</v>
+      </c>
+      <c r="M2">
+        <f>F2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5481,8 +4415,16 @@
         <f t="shared" ref="K3:K9" si="3">LN(J3*H3)</f>
         <v>-1.1711829815029451</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L9" si="4">(K3)^2</f>
+        <v>1.3716695761621278</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="5">F3*K3</f>
+        <v>-1.1711829815029451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5520,8 +4462,16 @@
         <f t="shared" si="3"/>
         <v>-0.60880603212619433</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>0.37064478475324075</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>-1.2176120642523887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5559,8 +4509,16 @@
         <f t="shared" si="3"/>
         <v>-7.9043207340452962E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>6.2478286266658368E-3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>-0.2371296220213589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5598,8 +4556,16 @@
         <f t="shared" si="3"/>
         <v>0.39743293641090011</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>0.15795293894419057</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1.5897317456436004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5637,8 +4603,16 @@
         <f t="shared" si="3"/>
         <v>0.87546873735389985</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>0.76644551008403172</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>4.3773436867694997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5676,8 +4650,16 @@
         <f t="shared" si="3"/>
         <v>1.9740810260220096</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>3.8969958973001102</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>11.844486156132058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5715,8 +4697,16 @@
         <f t="shared" si="3"/>
         <v>2.3105532626432224</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>5.3386563795112396</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>16.173872838502557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5733,7 +4723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5750,7 +4740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5767,7 +4757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5784,7 +4774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5801,7 +4791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5818,7 +4808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8477,15 +7467,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K501"/>
+  <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K8"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8519,8 +7509,14 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8558,8 +7554,16 @@
         <f>LN(J2*H2)</f>
         <v>-1.3547956940605197</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>(K2)^2</f>
+        <v>1.8354713726449252</v>
+      </c>
+      <c r="M2">
+        <f>F2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8597,8 +7601,16 @@
         <f t="shared" ref="K3:K8" si="3">LN(J3*H3)</f>
         <v>-1.0847093834991182</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="4">(K3)^2</f>
+        <v>1.176594446651037</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M8" si="5">F3*K3</f>
+        <v>-1.0847093834991182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8636,8 +7648,16 @@
         <f t="shared" si="3"/>
         <v>-0.67727383140365516</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>0.45869984270418673</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>-1.3545476628073103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8675,8 +7695,16 @@
         <f t="shared" si="3"/>
         <v>-0.41551544396166579</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>0.17265308417066022</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>-1.2465463318849974</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8714,8 +7742,16 @@
         <f t="shared" si="3"/>
         <v>-0.55164761828624564</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>0.30431509476088736</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>-2.2065904731449826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8753,8 +7789,16 @@
         <f t="shared" si="3"/>
         <v>0.51879379341516751</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>0.26914700008609949</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>2.5939689670758375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8792,8 +7836,16 @@
         <f t="shared" si="3"/>
         <v>0.36464311358790924</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>0.13296460028708487</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>2.1878586815274552</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8810,7 +7862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8827,7 +7879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8844,7 +7896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8861,7 +7913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8878,7 +7930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8895,7 +7947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8912,7 +7964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -17181,15 +16233,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K501"/>
+  <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K43"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17223,8 +16275,14 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -17262,8 +16320,16 @@
         <f>LN(J2*H2)</f>
         <v>104.79917879689515</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>(K2)^2</f>
+        <v>10982.867876503598</v>
+      </c>
+      <c r="M2">
+        <f>F2*K2</f>
+        <v>4191.9671518758059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -17301,8 +16367,16 @@
         <f t="shared" ref="K3:K43" si="3">LN(J3*H3)</f>
         <v>112.65588558999099</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L43" si="4">(K3)^2</f>
+        <v>12691.34855806514</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M43" si="5">F3*K3</f>
+        <v>4731.5471947796213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -17340,8 +16414,16 @@
         <f t="shared" si="3"/>
         <v>116.01162059757638</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>13458.696113676009</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>4988.4996856957841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -17379,8 +16461,16 @@
         <f t="shared" si="3"/>
         <v>124.00793782937313</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>15377.968644693672</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>5580.3572023217912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -17418,8 +16508,16 @@
         <f t="shared" si="3"/>
         <v>126.73796693719412</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>16062.512263373308</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>5829.9464791109294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -17457,8 +16555,16 @@
         <f t="shared" si="3"/>
         <v>132.19755245133828</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>17476.192874124336</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>6213.2849652128989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -17496,8 +16602,16 @@
         <f t="shared" si="3"/>
         <v>135.15246273037201</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>18266.188182084596</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>6487.3182110578564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -17535,8 +16649,16 @@
         <f t="shared" si="3"/>
         <v>140.74903112072107</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>19810.289761421707</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>6896.7025249153321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -17574,8 +16696,16 @@
         <f t="shared" si="3"/>
         <v>144.34260039503067</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>20834.786288799507</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>7217.1300197515338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -17613,8 +16743,16 @@
         <f t="shared" si="3"/>
         <v>148.274426027755</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>21985.305413860187</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>7561.9957274155049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -17652,8 +16790,16 @@
         <f t="shared" si="3"/>
         <v>152.0921383537119</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>23132.018549004642</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>7908.7911943930194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -17691,8 +16837,16 @@
         <f t="shared" si="3"/>
         <v>156.31374469554493</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>24433.986780743999</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>8284.6284688638807</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -17730,8 +16884,16 @@
         <f t="shared" si="3"/>
         <v>160.87809288701277</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>25881.760770962308</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>8687.417015898689</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -17769,8 +16931,16 @@
         <f t="shared" si="3"/>
         <v>165.33171317487367</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>27334.575381338695</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>9093.2442246180526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -17808,8 +16978,16 @@
         <f t="shared" si="3"/>
         <v>168.91077776298039</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>28530.850844494951</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>9459.0035547269017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -17847,8 +17025,16 @@
         <f t="shared" si="3"/>
         <v>173.40011613344336</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>30067.600275091645</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>9883.8066196062719</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -17886,8 +17072,16 @@
         <f t="shared" si="3"/>
         <v>177.3327257724799</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>31446.895629897557</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="5"/>
+        <v>10285.298094803835</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -17925,8 +17119,16 @@
         <f t="shared" si="3"/>
         <v>181.78495666582702</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="4"/>
+        <v>33045.770469996613</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="5"/>
+        <v>10725.312443283794</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -17964,8 +17166,16 @@
         <f t="shared" si="3"/>
         <v>185.18615404748917</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>34293.911650900387</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="5"/>
+        <v>11111.16924284935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -18003,8 +17213,16 @@
         <f t="shared" si="3"/>
         <v>189.65993340535186</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f t="shared" si="4"/>
+        <v>35970.890339322505</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="5"/>
+        <v>11569.255937726464</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -18042,8 +17260,16 @@
         <f t="shared" si="3"/>
         <v>193.69609601219122</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f t="shared" si="4"/>
+        <v>37518.177610364</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="5"/>
+        <v>12009.157952755855</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -18081,8 +17307,16 @@
         <f t="shared" si="3"/>
         <v>198.22869550534449</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f t="shared" si="4"/>
+        <v>39294.615721750582</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="5"/>
+        <v>12488.407816836703</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -18120,8 +17354,16 @@
         <f t="shared" si="3"/>
         <v>202.17246720908722</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="4"/>
+        <v>40873.706497409446</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="5"/>
+        <v>12939.037901381582</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -18159,8 +17401,16 @@
         <f t="shared" si="3"/>
         <v>206.17250109183806</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>42507.100206463962</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="5"/>
+        <v>13401.212570969474</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -18198,8 +17448,16 @@
         <f t="shared" si="3"/>
         <v>210.53650922100928</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>44325.621714968125</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="5"/>
+        <v>13895.409608586613</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -18237,8 +17495,16 @@
         <f t="shared" si="3"/>
         <v>214.35553935958825</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="4"/>
+        <v>45948.297254139987</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="5"/>
+        <v>14361.821137092413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -18276,8 +17542,16 @@
         <f t="shared" si="3"/>
         <v>218.51442244294793</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f t="shared" si="4"/>
+        <v>47748.552815575109</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="5"/>
+        <v>14858.980726120459</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -18315,8 +17589,16 @@
         <f t="shared" si="3"/>
         <v>222.7485289475452</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f t="shared" si="4"/>
+        <v>49616.90714829538</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="5"/>
+        <v>15369.648497380618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -18354,8 +17636,16 @@
         <f t="shared" si="3"/>
         <v>227.05764881141098</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="4"/>
+        <v>51555.175883766045</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="5"/>
+        <v>15894.03541679877</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -18393,8 +17683,16 @@
         <f t="shared" si="3"/>
         <v>231.0520647018576</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f t="shared" si="4"/>
+        <v>53385.05660299139</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="5"/>
+        <v>16404.69659383189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -18432,8 +17730,16 @@
         <f t="shared" si="3"/>
         <v>235.24868811320013</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f t="shared" si="4"/>
+        <v>55341.945258981708</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="5"/>
+        <v>16937.90554415041</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -18471,8 +17777,16 @@
         <f t="shared" si="3"/>
         <v>238.66367881699463</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <f t="shared" si="4"/>
+        <v>56960.351586461569</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="5"/>
+        <v>17422.448553640606</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -18510,8 +17824,16 @@
         <f t="shared" si="3"/>
         <v>243.30421614682001</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="4"/>
+        <v>59196.941594818512</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="5"/>
+        <v>18004.511994864682</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -18549,8 +17871,16 @@
         <f t="shared" si="3"/>
         <v>247.46755358052906</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="4"/>
+        <v>61240.190075132021</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="5"/>
+        <v>18560.066518539679</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -18588,8 +17918,16 @@
         <f t="shared" si="3"/>
         <v>252.08596899326716</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="4"/>
+        <v>63547.335763274452</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>19158.533643488303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -18627,8 +17965,16 @@
         <f t="shared" si="3"/>
         <v>256.42977441512085</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <f t="shared" si="4"/>
+        <v>65756.229206589764</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="5"/>
+        <v>19745.092629964303</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -18666,8 +18012,16 @@
         <f t="shared" si="3"/>
         <v>259.40018888069056</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <f t="shared" si="4"/>
+        <v>67288.457991337942</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="5"/>
+        <v>20233.214732693865</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -18705,8 +18059,16 @@
         <f t="shared" si="3"/>
         <v>265.02239970165294</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <f t="shared" si="4"/>
+        <v>70236.872343622701</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="5"/>
+        <v>20936.769576430583</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -18744,8 +18106,16 @@
         <f t="shared" si="3"/>
         <v>267.45851618727153</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <f t="shared" si="4"/>
+        <v>71534.057881096989</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="5"/>
+        <v>21396.681294981721</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -18783,8 +18153,16 @@
         <f t="shared" si="3"/>
         <v>272.95157763061206</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <f t="shared" si="4"/>
+        <v>74502.563731040049</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="5"/>
+        <v>22109.077788079576</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -18822,8 +18200,16 @@
         <f t="shared" si="3"/>
         <v>276.25968458920818</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f t="shared" si="4"/>
+        <v>76319.413329328789</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="5"/>
+        <v>22653.294136315071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -18861,8 +18247,16 @@
         <f t="shared" si="3"/>
         <v>281.37167237756472</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <f t="shared" si="4"/>
+        <v>79170.018016547619</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="5"/>
+        <v>23353.848807337872</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -18879,7 +18273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -18896,7 +18290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -18913,7 +18307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -18930,7 +18324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -26656,10 +26050,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K501"/>
+  <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26667,7 +26061,7 @@
     <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26701,8 +26095,14 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -26740,8 +26140,16 @@
         <f>LN(J2*H2)</f>
         <v>-5.521460917862246</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>(K2)^2</f>
+        <v>30.486530667480196</v>
+      </c>
+      <c r="M2">
+        <f>F2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -26779,8 +26187,16 @@
         <f t="shared" ref="K3:K17" si="3">LN(J3*H3)</f>
         <v>-4.6051701859880909</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L17" si="4">(K3)^2</f>
+        <v>21.207592441913587</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M17" si="5">F3*K3</f>
+        <v>-4.6051701859880909</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -26818,8 +26234,16 @@
         <f t="shared" si="3"/>
         <v>-2.6882475738060303</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>7.2266750180740082</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>-5.3764951476120606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -26857,8 +26281,16 @@
         <f t="shared" si="3"/>
         <v>-0.92634106772765645</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>0.85810777375881464</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>-2.7790232031829696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -26896,8 +26328,16 @@
         <f t="shared" si="3"/>
         <v>1.0409831758314734</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>1.0836459723641803</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>4.1639327033258935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -26935,8 +26375,16 @@
         <f t="shared" si="3"/>
         <v>3.0946722214088944</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>9.5769961579598615</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>15.473361107044472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -26974,8 +26422,16 @@
         <f t="shared" si="3"/>
         <v>4.9185200051884506</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>24.191839041438996</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>29.511120031130702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -27013,8 +26469,16 @@
         <f t="shared" si="3"/>
         <v>6.48494053253886</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>42.054453710565397</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>45.394583727772023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -27034,7 +26498,7 @@
         <v>8</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G17" si="4">F10^2</f>
+        <f t="shared" ref="G10:G17" si="6">F10^2</f>
         <v>64</v>
       </c>
       <c r="H10">
@@ -27052,8 +26516,16 @@
         <f t="shared" si="3"/>
         <v>8.3789788508873322</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>70.207286583617204</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="5"/>
+        <v>67.031830807098657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -27073,7 +26545,7 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>81</v>
       </c>
       <c r="H11">
@@ -27091,8 +26563,16 @@
         <f t="shared" si="3"/>
         <v>9.8830562476636068</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>97.67480079448265</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="5"/>
+        <v>88.947506228972458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -27112,7 +26592,7 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="H12">
@@ -27130,8 +26610,16 @@
         <f t="shared" si="3"/>
         <v>11.834243453819765</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>140.04931812427594</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="5"/>
+        <v>118.34243453819765</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -27151,7 +26639,7 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>121</v>
       </c>
       <c r="H13">
@@ -27169,8 +26657,16 @@
         <f t="shared" si="3"/>
         <v>14.46575357779964</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>209.25802657362308</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>159.12328935579603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -27190,7 +26686,7 @@
         <v>12</v>
       </c>
       <c r="G14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>144</v>
       </c>
       <c r="H14">
@@ -27208,8 +26704,16 @@
         <f t="shared" si="3"/>
         <v>14.871218685907804</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>221.15314520409345</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>178.45462423089364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -27229,7 +26733,7 @@
         <v>13</v>
       </c>
       <c r="G15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>169</v>
       </c>
       <c r="H15">
@@ -27247,8 +26751,16 @@
         <f t="shared" si="3"/>
         <v>17.436168043369342</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="4"/>
+        <v>304.0199560366143</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>226.67018456380146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -27268,7 +26780,7 @@
         <v>14</v>
       </c>
       <c r="G16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>196</v>
       </c>
       <c r="H16">
@@ -27286,8 +26798,16 @@
         <f t="shared" si="3"/>
         <v>18.97661308431649</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>360.11184415185181</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="5"/>
+        <v>265.67258318043088</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -27307,7 +26827,7 @@
         <v>15</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>225</v>
       </c>
       <c r="H17">
@@ -27325,8 +26845,16 @@
         <f t="shared" si="3"/>
         <v>21.684663285418701</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>470.22462180198573</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>325.2699492812805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -27343,7 +26871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -27360,7 +26888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -27377,7 +26905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -27394,7 +26922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -27411,7 +26939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -27428,7 +26956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -27445,7 +26973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -27462,7 +26990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -27479,7 +27007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -27496,7 +27024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -27513,7 +27041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -27530,7 +27058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -27547,7 +27075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -27564,7 +27092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -35561,18 +35089,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K501"/>
+  <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K1" activeCellId="1" sqref="F1:F9 K1:K9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35606,8 +35135,14 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -35645,8 +35180,16 @@
         <f>LN(J2*H2)</f>
         <v>-1.8971199848858813</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>(K2)^2</f>
+        <v>3.5990642370534065</v>
+      </c>
+      <c r="M2">
+        <f>F2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -35684,8 +35227,16 @@
         <f t="shared" ref="K3:K9" si="3">LN(J3*H3)</f>
         <v>-1.3318061758358208</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L9" si="4">(K3)^2</f>
+        <v>1.7737076899944333</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M9" si="5">F3*K3</f>
+        <v>-1.3318061758358208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -35723,8 +35274,16 @@
         <f t="shared" si="3"/>
         <v>-0.53102833108351022</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="4"/>
+        <v>0.28199108841333814</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="5"/>
+        <v>-1.0620566621670204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -35762,8 +35321,16 @@
         <f t="shared" si="3"/>
         <v>0.10975086395911929</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>1.2045252139773109E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>0.32925259187735789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -35801,8 +35368,16 @@
         <f t="shared" si="3"/>
         <v>0.33074156191222798</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>0.10938998077614014</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>1.3229662476489119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -35840,8 +35415,16 @@
         <f t="shared" si="3"/>
         <v>1.5173226235262947</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>2.3022679438647176</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>7.5866131176314733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -35879,8 +35462,16 @@
         <f t="shared" si="3"/>
         <v>1.7509374747077999</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>3.0657820403361273</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>10.5056248482468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -35918,8 +35509,16 @@
         <f t="shared" si="3"/>
         <v>4.3899948043230586</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>19.272054381983448</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="5"/>
+        <v>35.119958434584468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -35936,7 +35535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -35953,7 +35552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -35970,7 +35569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -35987,7 +35586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -36004,7 +35603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -36021,7 +35620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -44285,6 +43884,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>